<commit_message>
Transferências de colaboradores e correções em nomes.
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IE.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IE.XLSX
@@ -130,13 +130,13 @@
     <t>Domingo</t>
   </si>
   <si>
-    <t>PATRCIA APICELO</t>
+    <t>PATRICIA APICELO</t>
   </si>
   <si>
     <t>TAINNA PADELA BRAGA</t>
   </si>
   <si>
-    <t>RAFAEL DE SA DOS SANTOS</t>
+    <t>RAPHAEL DE SA DOS SANTOS</t>
   </si>
   <si>
     <t> </t>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="M12" s="174" t="str">
         <f>G12</f>
-        <v>PATRCIA APICELO</v>
+        <v>PATRICIA APICELO</v>
       </c>
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="P12" s="161" t="str">
         <f>I12</f>
-        <v>RAFAEL DE SA DOS SANTOS</v>
+        <v>RAPHAEL DE SA DOS SANTOS</v>
       </c>
       <c r="Q12" s="161" t="str">
         <f>J12</f>
@@ -3544,7 +3544,7 @@
       <c r="T12" s="189"/>
       <c r="U12" s="174" t="str">
         <f>G12</f>
-        <v>PATRCIA APICELO</v>
+        <v>PATRICIA APICELO</v>
       </c>
       <c r="V12" s="161"/>
       <c r="W12" s="161"/>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="Y12" s="161" t="str">
         <f>I12</f>
-        <v>RAFAEL DE SA DOS SANTOS</v>
+        <v>RAPHAEL DE SA DOS SANTOS</v>
       </c>
       <c r="Z12" s="161" t="str">
         <f>J12</f>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="AC12" s="181" t="str">
         <f t="shared" ref="AC12:AH12" si="0">G12</f>
-        <v>PATRCIA APICELO</v>
+        <v>PATRICIA APICELO</v>
       </c>
       <c r="AD12" s="183" t="str">
         <f t="shared" si="0"/>
@@ -3578,7 +3578,7 @@
       </c>
       <c r="AE12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v>RAFAEL DE SA DOS SANTOS</v>
+        <v>RAPHAEL DE SA DOS SANTOS</v>
       </c>
       <c r="AF12" s="161" t="str">
         <f t="shared" si="0"/>
@@ -3594,7 +3594,7 @@
       </c>
       <c r="AI12" s="185" t="str">
         <f t="shared" ref="AI12:AN12" si="1">G12</f>
-        <v>PATRCIA APICELO</v>
+        <v>PATRICIA APICELO</v>
       </c>
       <c r="AJ12" s="183" t="str">
         <f t="shared" si="1"/>
@@ -3602,7 +3602,7 @@
       </c>
       <c r="AK12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>RAFAEL DE SA DOS SANTOS</v>
+        <v>RAPHAEL DE SA DOS SANTOS</v>
       </c>
       <c r="AL12" s="161" t="str">
         <f t="shared" si="1"/>
@@ -6603,7 +6603,7 @@
       <c r="F12" s="159"/>
       <c r="G12" s="174" t="str">
         <f>'Segunda a Sexta'!G12:G18</f>
-        <v>PATRCIA APICELO</v>
+        <v>PATRICIA APICELO</v>
       </c>
       <c r="H12" s="161" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
@@ -6611,7 +6611,7 @@
       </c>
       <c r="I12" s="161" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v>RAFAEL DE SA DOS SANTOS</v>
+        <v>RAPHAEL DE SA DOS SANTOS</v>
       </c>
       <c r="J12" s="161" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="M12" s="174" t="str">
         <f>'Segunda a Sexta'!G12:G18</f>
-        <v>PATRCIA APICELO</v>
+        <v>PATRICIA APICELO</v>
       </c>
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
@@ -6636,7 +6636,7 @@
       </c>
       <c r="P12" s="187" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v>RAFAEL DE SA DOS SANTOS</v>
+        <v>RAPHAEL DE SA DOS SANTOS</v>
       </c>
       <c r="Q12" s="187" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>

</xml_diff>